<commit_message>
feat: Navigation between views
</commit_message>
<xml_diff>
--- a/Docs/TodoList.xlsx
+++ b/Docs/TodoList.xlsx
@@ -322,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -376,6 +376,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -391,32 +418,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -725,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,93 +755,93 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="21" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="27" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="27" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="27" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="30" t="s">
+      <c r="A8" s="29"/>
+      <c r="B8" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="32" t="s">
+      <c r="C8" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
@@ -850,7 +853,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
@@ -862,19 +865,19 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="C11" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="30" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -888,43 +891,43 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>9</v>
+      <c r="C13" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="31"/>
+      <c r="B14" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>9</v>
+      <c r="C14" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="31"/>
+      <c r="B15" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>9</v>
+      <c r="C15" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="28" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="18" t="s">
@@ -938,7 +941,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
@@ -950,7 +953,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
@@ -962,7 +965,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
@@ -974,7 +977,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="18" t="s">
@@ -988,7 +991,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="4" t="s">
         <v>30</v>
       </c>
@@ -1000,7 +1003,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="4" t="s">
         <v>33</v>
       </c>
@@ -1012,7 +1015,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="4" t="s">
         <v>31</v>
       </c>
@@ -1024,7 +1027,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="4" t="s">
         <v>32</v>
       </c>
@@ -1036,7 +1039,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="28" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="18" t="s">
@@ -1050,7 +1053,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="4" t="s">
         <v>36</v>
       </c>
@@ -1062,7 +1065,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="17" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
feat: Show Image and Return to back screen
</commit_message>
<xml_diff>
--- a/Docs/TodoList.xlsx
+++ b/Docs/TodoList.xlsx
@@ -322,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -338,9 +338,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -403,6 +400,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -417,9 +417,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -728,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,16 +738,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
     </row>
@@ -758,85 +755,85 @@
       <c r="A2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="29"/>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="27" t="s">
+      <c r="C8" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="26" t="s">
         <v>9</v>
       </c>
     </row>
@@ -845,10 +842,10 @@
       <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -857,22 +854,22 @@
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29"/>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="23" t="s">
         <v>9</v>
       </c>
     </row>
@@ -880,49 +877,49 @@
       <c r="A12" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>9</v>
+      <c r="C12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="31"/>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31"/>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>38</v>
       </c>
     </row>
@@ -930,13 +927,13 @@
       <c r="A16" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -945,10 +942,10 @@
       <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="C17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -957,10 +954,10 @@
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="10" t="s">
+      <c r="C18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -969,10 +966,10 @@
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="10" t="s">
+      <c r="C19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -980,13 +977,13 @@
       <c r="A20" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="C20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -995,10 +992,10 @@
       <c r="B21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="10" t="s">
+      <c r="C21" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1007,10 +1004,10 @@
       <c r="B22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="C22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1019,10 +1016,10 @@
       <c r="B23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1031,10 +1028,10 @@
       <c r="B24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="C24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1042,13 +1039,13 @@
       <c r="A25" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="8" t="s">
+      <c r="C25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1057,22 +1054,22 @@
       <c r="B26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="C26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="32"/>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="12" t="s">
+      <c r="C27" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Add Map to Office view
</commit_message>
<xml_diff>
--- a/Docs/TodoList.xlsx
+++ b/Docs/TodoList.xlsx
@@ -322,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -417,6 +417,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -725,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,10 +870,10 @@
         <v>17</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -927,14 +930,14 @@
       <c r="A16" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>9</v>
+      <c r="C16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -977,62 +980,62 @@
       <c r="A20" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>9</v>
+      <c r="C20" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="29"/>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>9</v>
+      <c r="C21" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="C22" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>9</v>
+      <c r="C23" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="29"/>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>9</v>
+      <c r="C24" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">

</xml_diff>